<commit_message>
updated collection to avoid false positives
</commit_message>
<xml_diff>
--- a/docs/Codebook_climate_change_stance_EN.xlsx
+++ b/docs/Codebook_climate_change_stance_EN.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lheyerda/Documents/GitHub/SICSS_EcoVibe/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DCBB54C-A713-1942-AD61-5E928975FB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9F1B74-5888-7441-AECC-49831F8E567B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{8A626D3D-B62E-BE4A-B8F8-982BE301115F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="EN" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -588,7 +588,7 @@
   <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>